<commit_message>
add languages and change to select policy
</commit_message>
<xml_diff>
--- a/src/locales/languages.xlsx
+++ b/src/locales/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/projects/hieunm/tax-calculator/src/locales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7058CC6B-A2EB-B148-86F3-F0C467FFFD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EA5C79-E14B-0942-B775-3B3F965ABFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="27320" windowHeight="14240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="187">
   <si>
     <t>Key</t>
   </si>
@@ -201,30 +201,9 @@
     <t>{0} に計算します</t>
   </si>
   <si>
-    <t>home.setting-button.label</t>
-  </si>
-  <si>
-    <t>Tax configuration</t>
-  </si>
-  <si>
-    <t>Cấu hình thuế</t>
-  </si>
-  <si>
-    <t>税金の設定</t>
-  </si>
-  <si>
     <t>home.alert.title</t>
   </si>
   <si>
-    <t>Notification</t>
-  </si>
-  <si>
-    <t>Thông báo</t>
-  </si>
-  <si>
-    <t>通知</t>
-  </si>
-  <si>
     <t>Mức bảo hiểm đã đóng là {0}₫</t>
   </si>
   <si>
@@ -294,18 +273,6 @@
     <t>個人控除</t>
   </si>
   <si>
-    <t>config.personal-deduction.placeholder</t>
-  </si>
-  <si>
-    <t>Enter personal deduction</t>
-  </si>
-  <si>
-    <t>Nhập giảm trừ cá nhân</t>
-  </si>
-  <si>
-    <t>個人控除を入力</t>
-  </si>
-  <si>
     <t>config.dependants-deduction.label</t>
   </si>
   <si>
@@ -318,18 +285,6 @@
     <t>扶養控除</t>
   </si>
   <si>
-    <t>config.dependants-deduction.placeholder</t>
-  </si>
-  <si>
-    <t>Enter dependants deduction</t>
-  </si>
-  <si>
-    <t>Nhập giảm trừ người phụ thuộc</t>
-  </si>
-  <si>
-    <t>扶養控除を入力</t>
-  </si>
-  <si>
     <t>config.insurance-rate.label</t>
   </si>
   <si>
@@ -354,72 +309,12 @@
     <t>最低保険基盤</t>
   </si>
   <si>
-    <t>config.save.label</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>Lưu</t>
-  </si>
-  <si>
-    <t>保存</t>
-  </si>
-  <si>
-    <t>config.default.label</t>
-  </si>
-  <si>
-    <t>Reset to default</t>
-  </si>
-  <si>
-    <t>Mặc định</t>
-  </si>
-  <si>
-    <t>デフォルトにリセット</t>
-  </si>
-  <si>
     <t>config.close.label</t>
   </si>
   <si>
-    <t>config.add-step.label</t>
-  </si>
-  <si>
-    <t>Thêm bậc</t>
-  </si>
-  <si>
-    <t>Add step</t>
-  </si>
-  <si>
-    <t>税金のステップを追加</t>
-  </si>
-  <si>
     <t>税引前所得は{0}₫です</t>
   </si>
   <si>
-    <t>config.tax-step-x.label</t>
-  </si>
-  <si>
-    <t>config.tax-rate-x.label</t>
-  </si>
-  <si>
-    <t>Tax step level {0}</t>
-  </si>
-  <si>
-    <t>Tax rate level {0}</t>
-  </si>
-  <si>
-    <t>Biểu thuế mức {0}</t>
-  </si>
-  <si>
-    <t>Tỷ suất thuế mức {0}</t>
-  </si>
-  <si>
-    <t>税段階レベル {0}</t>
-  </si>
-  <si>
-    <t>税率レベル {0}</t>
-  </si>
-  <si>
     <t>Gross income is {0}₫</t>
   </si>
   <si>
@@ -478,6 +373,219 @@
   </si>
   <si>
     <t>home.answer.row-6</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>필수 입력 항목</t>
+  </si>
+  <si>
+    <t>개인 소득세 스프레드시트</t>
+  </si>
+  <si>
+    <t>소득</t>
+  </si>
+  <si>
+    <t>소득 입력</t>
+  </si>
+  <si>
+    <t>부양가족 수</t>
+  </si>
+  <si>
+    <t>부양가족 수 입력</t>
+  </si>
+  <si>
+    <t>보험료 납부 수준</t>
+  </si>
+  <si>
+    <t>공무원 급여 초과</t>
+  </si>
+  <si>
+    <t>기타</t>
+  </si>
+  <si>
+    <t>최저 {0}₫</t>
+  </si>
+  <si>
+    <t>계산할 급여</t>
+  </si>
+  <si>
+    <t>순소득</t>
+  </si>
+  <si>
+    <t>총소득</t>
+  </si>
+  <si>
+    <t>급여 {0} 계산</t>
+  </si>
+  <si>
+    <t>총소득은 {0}₫입니다.</t>
+  </si>
+  <si>
+    <t>납부한 보험료는 {0}₫입니다.</t>
+  </si>
+  <si>
+    <t>세전 소득은 {0}₫입니다.</t>
+  </si>
+  <si>
+    <t>과세 소득은 {0}₫입니다.</t>
+  </si>
+  <si>
+    <t>납부할 세액은 {0}₫입니다.</t>
+  </si>
+  <si>
+    <t>순소득은 {0}₫입니다.</t>
+  </si>
+  <si>
+    <t>설정</t>
+  </si>
+  <si>
+    <t>언어</t>
+  </si>
+  <si>
+    <t>다크 모드</t>
+  </si>
+  <si>
+    <t>닫기</t>
+  </si>
+  <si>
+    <t>개인 공제</t>
+  </si>
+  <si>
+    <t>부양가족 공제</t>
+  </si>
+  <si>
+    <t>보험료 납부율</t>
+  </si>
+  <si>
+    <t>최저 급여</t>
+  </si>
+  <si>
+    <t>Tax step</t>
+  </si>
+  <si>
+    <t>Biểu thuế</t>
+  </si>
+  <si>
+    <t>Tax rate</t>
+  </si>
+  <si>
+    <t>Tỷ suất thuế</t>
+  </si>
+  <si>
+    <t>税金のステップ</t>
+  </si>
+  <si>
+    <t>税率</t>
+  </si>
+  <si>
+    <t>세금 단계</t>
+  </si>
+  <si>
+    <t>세율</t>
+  </si>
+  <si>
+    <t>config.tax-step.label</t>
+  </si>
+  <si>
+    <t>config.tax-rate.label</t>
+  </si>
+  <si>
+    <t>config.tax-level.label</t>
+  </si>
+  <si>
+    <t>Tax level</t>
+  </si>
+  <si>
+    <t>Bậc</t>
+  </si>
+  <si>
+    <t>세금 수준</t>
+  </si>
+  <si>
+    <t>config.policy.label</t>
+  </si>
+  <si>
+    <t>법률 제04/2007/QH12호</t>
+  </si>
+  <si>
+    <t>Luật số 04/2007/QH12</t>
+  </si>
+  <si>
+    <t>config.policy.label1</t>
+  </si>
+  <si>
+    <t>config.policy.label2</t>
+  </si>
+  <si>
+    <t>config.policy.label3</t>
+  </si>
+  <si>
+    <t>Nghị quyết 954/2020/UBTVQH14</t>
+  </si>
+  <si>
+    <t>Nghị quyết 110/2025/UBTVQH15</t>
+  </si>
+  <si>
+    <t>決議110/2025/UBTVQH15</t>
+  </si>
+  <si>
+    <t>決議954/2020/UBTVQH14</t>
+  </si>
+  <si>
+    <t>결의안 954/2020/UBTVQH14</t>
+  </si>
+  <si>
+    <t>결의안 110/2025/UBTVQH15</t>
+  </si>
+  <si>
+    <t>Law No. 04/2007/QH12</t>
+  </si>
+  <si>
+    <t>Resolution 954/2020/UBTVQH14</t>
+  </si>
+  <si>
+    <t>Resolution 110/2025/UBTVQH15</t>
+  </si>
+  <si>
+    <t>Chính sách thuế TNCN</t>
+  </si>
+  <si>
+    <t>PIT Policy</t>
+  </si>
+  <si>
+    <t>個人所得税政策</t>
+  </si>
+  <si>
+    <t>개인소득세 정책</t>
+  </si>
+  <si>
+    <t>config.policy.tooltip</t>
+  </si>
+  <si>
+    <t>Tax policy detail</t>
+  </si>
+  <si>
+    <t>Chi tiết chính sách thuế</t>
+  </si>
+  <si>
+    <t>세금 정책 세부 정보</t>
+  </si>
+  <si>
+    <t>税制の詳細</t>
+  </si>
+  <si>
+    <t>Chi tiết lương và thuế</t>
+  </si>
+  <si>
+    <t>Salary and tax detail</t>
+  </si>
+  <si>
+    <t>給与と税金の詳細</t>
+  </si>
+  <si>
+    <t>급여 및 세금 세부 정보</t>
   </si>
 </sst>
 </file>
@@ -753,22 +861,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D486"/>
+  <dimension ref="A1:E486"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="42.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -781,8 +890,11 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E1" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -795,8 +907,11 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E2" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -809,8 +924,11 @@
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E3" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -823,8 +941,11 @@
       <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E4" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -837,8 +958,11 @@
       <c r="D5" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E5" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -851,8 +975,11 @@
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E6" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -865,8 +992,11 @@
       <c r="D7" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E7" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -879,8 +1009,11 @@
       <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E8" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -893,8 +1026,11 @@
       <c r="D9" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E9" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -907,8 +1043,11 @@
       <c r="D10" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E10" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
@@ -921,8 +1060,11 @@
       <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E11" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -935,8 +1077,11 @@
       <c r="D12" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E12" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
@@ -949,8 +1094,11 @@
       <c r="D13" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="E13" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -963,8 +1111,11 @@
       <c r="D14" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="E14" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -977,8 +1128,11 @@
       <c r="D15" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E15" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
@@ -991,3014 +1145,3089 @@
       <c r="D16" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="E16" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E22" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="E23" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="E24" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="D38" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="D39" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="E39" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
     </row>
-    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
-    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
-    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
     </row>
-    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
     </row>
-    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
     </row>
-    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
     </row>
-    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
     </row>
-    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
     </row>
-    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
     </row>
-    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
     </row>
-    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
     </row>
-    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
     </row>
-    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
     </row>
-    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
     </row>
-    <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
     </row>
-    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
     </row>
-    <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
     </row>
-    <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
     </row>
-    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
     </row>
-    <row r="109" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
     </row>
-    <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
     </row>
-    <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
     </row>
-    <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
     </row>
-    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
     </row>
-    <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
     </row>
-    <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
     </row>
-    <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
     </row>
-    <row r="118" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
     </row>
-    <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
     </row>
-    <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
     </row>
-    <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
     </row>
-    <row r="122" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
     </row>
-    <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
     </row>
-    <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
     </row>
-    <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
     </row>
-    <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
     </row>
-    <row r="127" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
     </row>
-    <row r="128" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
     </row>
-    <row r="129" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
     </row>
-    <row r="131" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
     </row>
-    <row r="133" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
     </row>
-    <row r="134" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
     </row>
-    <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
     </row>
-    <row r="136" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
     </row>
-    <row r="137" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
     </row>
-    <row r="140" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
     </row>
-    <row r="141" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
     </row>
-    <row r="142" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="3"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
     </row>
-    <row r="143" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="3"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
     </row>
-    <row r="144" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="3"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="3"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
     </row>
-    <row r="146" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="3"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
     </row>
-    <row r="147" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="3"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
     </row>
-    <row r="148" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
     </row>
-    <row r="150" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
     </row>
-    <row r="151" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
     </row>
-    <row r="152" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
     </row>
-    <row r="153" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
     </row>
-    <row r="154" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
     </row>
-    <row r="155" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
     </row>
-    <row r="156" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="3"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
     </row>
-    <row r="157" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="3"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
     </row>
-    <row r="158" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
     </row>
-    <row r="159" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="3"/>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
     </row>
-    <row r="160" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="3"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
     </row>
-    <row r="161" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="3"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
     </row>
-    <row r="162" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="3"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
     </row>
-    <row r="163" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="3"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
     </row>
-    <row r="164" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="3"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
     </row>
-    <row r="165" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
     </row>
-    <row r="166" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
     </row>
-    <row r="167" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="3"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
     </row>
-    <row r="168" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="3"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
     </row>
-    <row r="169" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="3"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
     </row>
-    <row r="170" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="3"/>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
     </row>
-    <row r="171" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="3"/>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
     </row>
-    <row r="172" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="3"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
     </row>
-    <row r="173" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="3"/>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
     </row>
-    <row r="174" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="3"/>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
     </row>
-    <row r="175" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="3"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
     </row>
-    <row r="176" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="3"/>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
     </row>
-    <row r="177" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="3"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
     </row>
-    <row r="178" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="3"/>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
       <c r="D178" s="4"/>
     </row>
-    <row r="179" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="3"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
       <c r="D179" s="4"/>
     </row>
-    <row r="180" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
     </row>
-    <row r="181" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
     </row>
-    <row r="182" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="3"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
       <c r="D182" s="4"/>
     </row>
-    <row r="183" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="3"/>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
       <c r="D183" s="4"/>
     </row>
-    <row r="184" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="3"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
       <c r="D184" s="4"/>
     </row>
-    <row r="185" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="3"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
       <c r="D185" s="4"/>
     </row>
-    <row r="186" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="3"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
       <c r="D186" s="4"/>
     </row>
-    <row r="187" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="3"/>
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
       <c r="D187" s="4"/>
     </row>
-    <row r="188" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="3"/>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
       <c r="D188" s="4"/>
     </row>
-    <row r="189" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="3"/>
       <c r="B189" s="6"/>
       <c r="C189" s="6"/>
       <c r="D189" s="4"/>
     </row>
-    <row r="190" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="3"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
     </row>
-    <row r="191" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="3"/>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
     </row>
-    <row r="192" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="3"/>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
       <c r="D192" s="4"/>
     </row>
-    <row r="193" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="3"/>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
       <c r="D193" s="4"/>
     </row>
-    <row r="194" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="3"/>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
       <c r="D194" s="4"/>
     </row>
-    <row r="195" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="3"/>
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
     </row>
-    <row r="196" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="3"/>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
       <c r="D196" s="4"/>
     </row>
-    <row r="197" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="3"/>
       <c r="B197" s="4"/>
       <c r="C197" s="4"/>
       <c r="D197" s="4"/>
     </row>
-    <row r="198" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="3"/>
       <c r="B198" s="6"/>
       <c r="C198" s="6"/>
       <c r="D198" s="4"/>
     </row>
-    <row r="199" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="3"/>
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
       <c r="D199" s="4"/>
     </row>
-    <row r="200" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="3"/>
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
       <c r="D200" s="4"/>
     </row>
-    <row r="201" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="3"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
       <c r="D201" s="4"/>
     </row>
-    <row r="202" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="3"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="4"/>
     </row>
-    <row r="203" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="3"/>
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
     </row>
-    <row r="204" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="3"/>
       <c r="B204" s="4"/>
       <c r="C204" s="4"/>
       <c r="D204" s="4"/>
     </row>
-    <row r="205" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="3"/>
       <c r="B205" s="4"/>
       <c r="C205" s="4"/>
       <c r="D205" s="4"/>
     </row>
-    <row r="206" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="3"/>
       <c r="B206" s="4"/>
       <c r="C206" s="4"/>
       <c r="D206" s="4"/>
     </row>
-    <row r="207" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="3"/>
       <c r="B207" s="4"/>
       <c r="C207" s="4"/>
       <c r="D207" s="4"/>
     </row>
-    <row r="208" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="3"/>
       <c r="B208" s="4"/>
       <c r="C208" s="4"/>
       <c r="D208" s="4"/>
     </row>
-    <row r="209" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="3"/>
       <c r="B209" s="4"/>
       <c r="C209" s="4"/>
       <c r="D209" s="4"/>
     </row>
-    <row r="210" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="3"/>
       <c r="B210" s="4"/>
       <c r="C210" s="4"/>
       <c r="D210" s="4"/>
     </row>
-    <row r="211" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="3"/>
       <c r="B211" s="4"/>
       <c r="C211" s="4"/>
       <c r="D211" s="4"/>
     </row>
-    <row r="212" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="3"/>
       <c r="B212" s="4"/>
       <c r="C212" s="4"/>
       <c r="D212" s="4"/>
     </row>
-    <row r="213" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="3"/>
       <c r="B213" s="4"/>
       <c r="C213" s="4"/>
       <c r="D213" s="4"/>
     </row>
-    <row r="214" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="3"/>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
     </row>
-    <row r="215" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="3"/>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
     </row>
-    <row r="216" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="3"/>
       <c r="B216" s="4"/>
       <c r="C216" s="4"/>
       <c r="D216" s="4"/>
     </row>
-    <row r="217" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="3"/>
       <c r="B217" s="4"/>
       <c r="C217" s="4"/>
       <c r="D217" s="4"/>
     </row>
-    <row r="218" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="3"/>
       <c r="B218" s="4"/>
       <c r="C218" s="4"/>
       <c r="D218" s="4"/>
     </row>
-    <row r="219" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="3"/>
       <c r="B219" s="4"/>
       <c r="C219" s="4"/>
       <c r="D219" s="4"/>
     </row>
-    <row r="220" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="3"/>
       <c r="B220" s="4"/>
       <c r="C220" s="4"/>
       <c r="D220" s="4"/>
     </row>
-    <row r="221" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="3"/>
       <c r="B221" s="4"/>
       <c r="C221" s="4"/>
       <c r="D221" s="4"/>
     </row>
-    <row r="222" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="3"/>
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
       <c r="D222" s="4"/>
     </row>
-    <row r="223" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="3"/>
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
       <c r="D223" s="4"/>
     </row>
-    <row r="224" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="3"/>
       <c r="B224" s="4"/>
       <c r="C224" s="4"/>
       <c r="D224" s="4"/>
     </row>
-    <row r="225" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="3"/>
       <c r="B225" s="4"/>
       <c r="C225" s="4"/>
       <c r="D225" s="4"/>
     </row>
-    <row r="226" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="3"/>
       <c r="B226" s="4"/>
       <c r="C226" s="4"/>
       <c r="D226" s="4"/>
     </row>
-    <row r="227" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="3"/>
       <c r="B227" s="4"/>
       <c r="C227" s="4"/>
       <c r="D227" s="4"/>
     </row>
-    <row r="228" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="3"/>
       <c r="B228" s="4"/>
       <c r="C228" s="4"/>
       <c r="D228" s="4"/>
     </row>
-    <row r="229" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="3"/>
       <c r="B229" s="4"/>
       <c r="C229" s="4"/>
       <c r="D229" s="4"/>
     </row>
-    <row r="230" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="3"/>
       <c r="B230" s="4"/>
       <c r="C230" s="4"/>
       <c r="D230" s="4"/>
     </row>
-    <row r="231" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="3"/>
       <c r="B231" s="4"/>
       <c r="C231" s="4"/>
       <c r="D231" s="4"/>
     </row>
-    <row r="232" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="3"/>
       <c r="B232" s="4"/>
       <c r="C232" s="4"/>
       <c r="D232" s="4"/>
     </row>
-    <row r="233" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="3"/>
       <c r="B233" s="4"/>
       <c r="C233" s="4"/>
       <c r="D233" s="4"/>
     </row>
-    <row r="234" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="3"/>
       <c r="B234" s="4"/>
       <c r="C234" s="4"/>
       <c r="D234" s="4"/>
     </row>
-    <row r="235" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="3"/>
       <c r="B235" s="4"/>
       <c r="C235" s="4"/>
       <c r="D235" s="4"/>
     </row>
-    <row r="236" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="3"/>
       <c r="B236" s="4"/>
       <c r="C236" s="4"/>
       <c r="D236" s="4"/>
     </row>
-    <row r="237" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="3"/>
       <c r="B237" s="4"/>
       <c r="C237" s="4"/>
       <c r="D237" s="4"/>
     </row>
-    <row r="238" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="3"/>
       <c r="B238" s="4"/>
       <c r="C238" s="4"/>
       <c r="D238" s="4"/>
     </row>
-    <row r="239" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="3"/>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
       <c r="D239" s="4"/>
     </row>
-    <row r="240" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="3"/>
       <c r="B240" s="4"/>
       <c r="C240" s="4"/>
       <c r="D240" s="4"/>
     </row>
-    <row r="241" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="3"/>
       <c r="B241" s="4"/>
       <c r="C241" s="4"/>
       <c r="D241" s="4"/>
     </row>
-    <row r="242" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="3"/>
       <c r="B242" s="4"/>
       <c r="C242" s="4"/>
       <c r="D242" s="4"/>
     </row>
-    <row r="243" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="3"/>
       <c r="B243" s="4"/>
       <c r="C243" s="4"/>
       <c r="D243" s="4"/>
     </row>
-    <row r="244" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="3"/>
       <c r="B244" s="4"/>
       <c r="C244" s="4"/>
       <c r="D244" s="4"/>
     </row>
-    <row r="245" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="3"/>
       <c r="B245" s="4"/>
       <c r="C245" s="4"/>
       <c r="D245" s="4"/>
     </row>
-    <row r="246" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="3"/>
       <c r="B246" s="4"/>
       <c r="C246" s="4"/>
       <c r="D246" s="4"/>
     </row>
-    <row r="247" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="3"/>
       <c r="B247" s="4"/>
       <c r="C247" s="4"/>
       <c r="D247" s="4"/>
     </row>
-    <row r="248" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="3"/>
       <c r="B248" s="4"/>
       <c r="C248" s="4"/>
       <c r="D248" s="4"/>
     </row>
-    <row r="249" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="3"/>
       <c r="B249" s="4"/>
       <c r="C249" s="4"/>
       <c r="D249" s="4"/>
     </row>
-    <row r="250" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="3"/>
       <c r="B250" s="4"/>
       <c r="C250" s="4"/>
       <c r="D250" s="4"/>
     </row>
-    <row r="251" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="3"/>
       <c r="B251" s="4"/>
       <c r="C251" s="4"/>
       <c r="D251" s="4"/>
     </row>
-    <row r="252" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="3"/>
       <c r="B252" s="4"/>
       <c r="C252" s="4"/>
       <c r="D252" s="4"/>
     </row>
-    <row r="253" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="3"/>
       <c r="B253" s="4"/>
       <c r="C253" s="4"/>
       <c r="D253" s="4"/>
     </row>
-    <row r="254" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="3"/>
       <c r="B254" s="4"/>
       <c r="C254" s="4"/>
       <c r="D254" s="4"/>
     </row>
-    <row r="255" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="3"/>
       <c r="B255" s="4"/>
       <c r="C255" s="4"/>
       <c r="D255" s="4"/>
     </row>
-    <row r="256" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="3"/>
       <c r="B256" s="4"/>
       <c r="C256" s="4"/>
       <c r="D256" s="4"/>
     </row>
-    <row r="257" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" s="3"/>
       <c r="B257" s="4"/>
       <c r="C257" s="4"/>
       <c r="D257" s="4"/>
     </row>
-    <row r="258" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" s="3"/>
       <c r="B258" s="4"/>
       <c r="C258" s="4"/>
       <c r="D258" s="4"/>
     </row>
-    <row r="259" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" s="3"/>
       <c r="B259" s="4"/>
       <c r="C259" s="4"/>
       <c r="D259" s="4"/>
     </row>
-    <row r="260" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" s="3"/>
       <c r="B260" s="4"/>
       <c r="C260" s="4"/>
       <c r="D260" s="4"/>
     </row>
-    <row r="261" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" s="3"/>
       <c r="B261" s="4"/>
       <c r="C261" s="4"/>
       <c r="D261" s="4"/>
     </row>
-    <row r="262" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="3"/>
       <c r="B262" s="4"/>
       <c r="C262" s="4"/>
       <c r="D262" s="4"/>
     </row>
-    <row r="263" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" s="3"/>
       <c r="B263" s="4"/>
       <c r="C263" s="4"/>
       <c r="D263" s="4"/>
     </row>
-    <row r="264" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="3"/>
       <c r="B264" s="4"/>
       <c r="C264" s="4"/>
       <c r="D264" s="4"/>
     </row>
-    <row r="265" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" s="3"/>
       <c r="B265" s="4"/>
       <c r="C265" s="4"/>
       <c r="D265" s="4"/>
     </row>
-    <row r="266" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" s="3"/>
       <c r="B266" s="4"/>
       <c r="C266" s="4"/>
       <c r="D266" s="4"/>
     </row>
-    <row r="267" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" s="3"/>
       <c r="B267" s="4"/>
       <c r="C267" s="4"/>
       <c r="D267" s="4"/>
     </row>
-    <row r="268" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" s="3"/>
       <c r="B268" s="4"/>
       <c r="C268" s="4"/>
       <c r="D268" s="4"/>
     </row>
-    <row r="269" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" s="3"/>
       <c r="B269" s="4"/>
       <c r="C269" s="4"/>
       <c r="D269" s="4"/>
     </row>
-    <row r="270" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" s="3"/>
       <c r="B270" s="4"/>
       <c r="C270" s="4"/>
       <c r="D270" s="4"/>
     </row>
-    <row r="271" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" s="3"/>
       <c r="B271" s="4"/>
       <c r="C271" s="4"/>
       <c r="D271" s="4"/>
     </row>
-    <row r="272" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" s="3"/>
       <c r="B272" s="4"/>
       <c r="C272" s="4"/>
       <c r="D272" s="4"/>
     </row>
-    <row r="273" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="3"/>
       <c r="B273" s="4"/>
       <c r="C273" s="4"/>
       <c r="D273" s="4"/>
     </row>
-    <row r="274" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" s="3"/>
       <c r="B274" s="4"/>
       <c r="C274" s="4"/>
       <c r="D274" s="4"/>
     </row>
-    <row r="275" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="3"/>
       <c r="B275" s="4"/>
       <c r="C275" s="4"/>
       <c r="D275" s="4"/>
     </row>
-    <row r="276" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="3"/>
       <c r="B276" s="4"/>
       <c r="C276" s="4"/>
       <c r="D276" s="4"/>
     </row>
-    <row r="277" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="3"/>
       <c r="B277" s="4"/>
       <c r="C277" s="4"/>
       <c r="D277" s="4"/>
     </row>
-    <row r="278" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="3"/>
       <c r="B278" s="4"/>
       <c r="C278" s="4"/>
       <c r="D278" s="4"/>
     </row>
-    <row r="279" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="3"/>
       <c r="B279" s="4"/>
       <c r="C279" s="4"/>
       <c r="D279" s="4"/>
     </row>
-    <row r="280" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="3"/>
       <c r="B280" s="4"/>
       <c r="C280" s="4"/>
       <c r="D280" s="4"/>
     </row>
-    <row r="281" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="3"/>
       <c r="B281" s="4"/>
       <c r="C281" s="4"/>
       <c r="D281" s="4"/>
     </row>
-    <row r="282" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="3"/>
       <c r="B282" s="4"/>
       <c r="C282" s="4"/>
       <c r="D282" s="4"/>
     </row>
-    <row r="283" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="3"/>
       <c r="B283" s="4"/>
       <c r="C283" s="4"/>
       <c r="D283" s="4"/>
     </row>
-    <row r="284" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="3"/>
       <c r="B284" s="4"/>
       <c r="C284" s="4"/>
       <c r="D284" s="4"/>
     </row>
-    <row r="285" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="3"/>
       <c r="B285" s="4"/>
       <c r="C285" s="4"/>
       <c r="D285" s="4"/>
     </row>
-    <row r="286" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" s="3"/>
       <c r="B286" s="4"/>
       <c r="C286" s="4"/>
       <c r="D286" s="4"/>
     </row>
-    <row r="287" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" s="3"/>
       <c r="B287" s="4"/>
       <c r="C287" s="4"/>
       <c r="D287" s="4"/>
     </row>
-    <row r="288" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" s="3"/>
       <c r="B288" s="4"/>
       <c r="C288" s="4"/>
       <c r="D288" s="4"/>
     </row>
-    <row r="289" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" s="3"/>
       <c r="B289" s="4"/>
       <c r="C289" s="4"/>
       <c r="D289" s="4"/>
     </row>
-    <row r="290" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" s="3"/>
       <c r="B290" s="4"/>
       <c r="C290" s="4"/>
       <c r="D290" s="4"/>
     </row>
-    <row r="291" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" s="3"/>
       <c r="B291" s="4"/>
       <c r="C291" s="4"/>
       <c r="D291" s="4"/>
     </row>
-    <row r="292" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" s="3"/>
       <c r="B292" s="4"/>
       <c r="C292" s="4"/>
       <c r="D292" s="4"/>
     </row>
-    <row r="293" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" s="3"/>
       <c r="B293" s="4"/>
       <c r="C293" s="4"/>
       <c r="D293" s="4"/>
     </row>
-    <row r="294" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" s="3"/>
       <c r="B294" s="4"/>
       <c r="C294" s="4"/>
       <c r="D294" s="4"/>
     </row>
-    <row r="295" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" s="3"/>
       <c r="B295" s="4"/>
       <c r="C295" s="4"/>
       <c r="D295" s="4"/>
     </row>
-    <row r="296" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" s="3"/>
       <c r="B296" s="4"/>
       <c r="C296" s="4"/>
       <c r="D296" s="4"/>
     </row>
-    <row r="297" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" s="3"/>
       <c r="B297" s="4"/>
       <c r="C297" s="4"/>
       <c r="D297" s="4"/>
     </row>
-    <row r="298" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" s="3"/>
       <c r="B298" s="4"/>
       <c r="C298" s="4"/>
       <c r="D298" s="4"/>
     </row>
-    <row r="299" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" s="3"/>
       <c r="B299" s="4"/>
       <c r="C299" s="4"/>
       <c r="D299" s="4"/>
     </row>
-    <row r="300" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" s="3"/>
       <c r="B300" s="4"/>
       <c r="C300" s="4"/>
       <c r="D300" s="4"/>
     </row>
-    <row r="301" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" s="3"/>
       <c r="B301" s="4"/>
       <c r="C301" s="4"/>
       <c r="D301" s="4"/>
     </row>
-    <row r="302" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" s="3"/>
       <c r="B302" s="4"/>
       <c r="C302" s="4"/>
       <c r="D302" s="4"/>
     </row>
-    <row r="303" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" s="3"/>
       <c r="B303" s="4"/>
       <c r="C303" s="4"/>
       <c r="D303" s="4"/>
     </row>
-    <row r="304" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" s="3"/>
       <c r="B304" s="4"/>
       <c r="C304" s="4"/>
       <c r="D304" s="4"/>
     </row>
-    <row r="305" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" s="3"/>
       <c r="B305" s="4"/>
       <c r="C305" s="4"/>
       <c r="D305" s="4"/>
     </row>
-    <row r="306" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" s="3"/>
       <c r="B306" s="4"/>
       <c r="C306" s="4"/>
       <c r="D306" s="4"/>
     </row>
-    <row r="307" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" s="3"/>
       <c r="B307" s="4"/>
       <c r="C307" s="4"/>
       <c r="D307" s="4"/>
     </row>
-    <row r="308" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" s="3"/>
       <c r="B308" s="4"/>
       <c r="C308" s="4"/>
       <c r="D308" s="4"/>
     </row>
-    <row r="309" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" s="3"/>
       <c r="B309" s="4"/>
       <c r="C309" s="4"/>
       <c r="D309" s="4"/>
     </row>
-    <row r="310" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" s="3"/>
       <c r="B310" s="4"/>
       <c r="C310" s="4"/>
       <c r="D310" s="4"/>
     </row>
-    <row r="311" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" s="3"/>
       <c r="B311" s="4"/>
       <c r="C311" s="4"/>
       <c r="D311" s="4"/>
     </row>
-    <row r="312" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" s="3"/>
       <c r="B312" s="4"/>
       <c r="C312" s="4"/>
       <c r="D312" s="4"/>
     </row>
-    <row r="313" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" s="3"/>
       <c r="B313" s="4"/>
       <c r="C313" s="4"/>
       <c r="D313" s="4"/>
     </row>
-    <row r="314" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" s="3"/>
       <c r="B314" s="4"/>
       <c r="C314" s="4"/>
       <c r="D314" s="4"/>
     </row>
-    <row r="315" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" s="3"/>
       <c r="B315" s="4"/>
       <c r="C315" s="4"/>
       <c r="D315" s="4"/>
     </row>
-    <row r="316" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316" s="3"/>
       <c r="B316" s="4"/>
       <c r="C316" s="4"/>
       <c r="D316" s="4"/>
     </row>
-    <row r="317" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317" s="3"/>
       <c r="B317" s="4"/>
       <c r="C317" s="4"/>
       <c r="D317" s="4"/>
     </row>
-    <row r="318" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318" s="3"/>
       <c r="B318" s="4"/>
       <c r="C318" s="4"/>
       <c r="D318" s="4"/>
     </row>
-    <row r="319" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319" s="3"/>
       <c r="B319" s="4"/>
       <c r="C319" s="4"/>
       <c r="D319" s="4"/>
     </row>
-    <row r="320" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320" s="3"/>
       <c r="B320" s="4"/>
       <c r="C320" s="4"/>
       <c r="D320" s="4"/>
     </row>
-    <row r="321" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321" s="3"/>
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
       <c r="D321" s="4"/>
     </row>
-    <row r="322" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A322" s="3"/>
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
       <c r="D322" s="4"/>
     </row>
-    <row r="323" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323" s="3"/>
       <c r="B323" s="4"/>
       <c r="C323" s="4"/>
       <c r="D323" s="4"/>
     </row>
-    <row r="324" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324" s="3"/>
       <c r="B324" s="4"/>
       <c r="C324" s="4"/>
       <c r="D324" s="4"/>
     </row>
-    <row r="325" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325" s="3"/>
       <c r="B325" s="4"/>
       <c r="C325" s="4"/>
       <c r="D325" s="4"/>
     </row>
-    <row r="326" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" s="3"/>
       <c r="B326" s="4"/>
       <c r="C326" s="4"/>
       <c r="D326" s="4"/>
     </row>
-    <row r="327" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" s="3"/>
       <c r="B327" s="4"/>
       <c r="C327" s="4"/>
       <c r="D327" s="4"/>
     </row>
-    <row r="328" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328" s="3"/>
       <c r="B328" s="4"/>
       <c r="C328" s="4"/>
       <c r="D328" s="4"/>
     </row>
-    <row r="329" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329" s="3"/>
       <c r="B329" s="4"/>
       <c r="C329" s="4"/>
       <c r="D329" s="4"/>
     </row>
-    <row r="330" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330" s="3"/>
       <c r="B330" s="4"/>
       <c r="C330" s="4"/>
       <c r="D330" s="4"/>
     </row>
-    <row r="331" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A331" s="3"/>
       <c r="B331" s="4"/>
       <c r="C331" s="4"/>
       <c r="D331" s="4"/>
     </row>
-    <row r="332" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A332" s="3"/>
       <c r="B332" s="4"/>
       <c r="C332" s="4"/>
       <c r="D332" s="4"/>
     </row>
-    <row r="333" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A333" s="3"/>
       <c r="B333" s="4"/>
       <c r="C333" s="4"/>
       <c r="D333" s="4"/>
     </row>
-    <row r="334" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A334" s="3"/>
       <c r="B334" s="4"/>
       <c r="C334" s="4"/>
       <c r="D334" s="4"/>
     </row>
-    <row r="335" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A335" s="3"/>
       <c r="B335" s="4"/>
       <c r="C335" s="4"/>
       <c r="D335" s="4"/>
     </row>
-    <row r="336" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A336" s="3"/>
       <c r="B336" s="4"/>
       <c r="C336" s="4"/>
       <c r="D336" s="4"/>
     </row>
-    <row r="337" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A337" s="3"/>
       <c r="B337" s="4"/>
       <c r="C337" s="4"/>
       <c r="D337" s="4"/>
     </row>
-    <row r="338" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338" s="3"/>
       <c r="B338" s="4"/>
       <c r="C338" s="4"/>
       <c r="D338" s="4"/>
     </row>
-    <row r="339" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A339" s="3"/>
       <c r="B339" s="4"/>
       <c r="C339" s="4"/>
       <c r="D339" s="4"/>
     </row>
-    <row r="340" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A340" s="3"/>
       <c r="B340" s="4"/>
       <c r="C340" s="4"/>
       <c r="D340" s="4"/>
     </row>
-    <row r="341" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A341" s="3"/>
       <c r="B341" s="4"/>
       <c r="C341" s="4"/>
       <c r="D341" s="4"/>
     </row>
-    <row r="342" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A342" s="3"/>
       <c r="B342" s="3"/>
       <c r="C342" s="4"/>
       <c r="D342" s="4"/>
     </row>
-    <row r="343" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A343" s="3"/>
       <c r="B343" s="4"/>
       <c r="C343" s="4"/>
       <c r="D343" s="4"/>
     </row>
-    <row r="344" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A344" s="3"/>
       <c r="B344" s="4"/>
       <c r="C344" s="4"/>
       <c r="D344" s="4"/>
     </row>
-    <row r="345" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A345" s="3"/>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
       <c r="D345" s="4"/>
     </row>
-    <row r="346" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A346" s="3"/>
       <c r="B346" s="4"/>
       <c r="C346" s="4"/>
       <c r="D346" s="4"/>
     </row>
-    <row r="347" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347" s="3"/>
       <c r="B347" s="4"/>
       <c r="C347" s="4"/>
       <c r="D347" s="4"/>
     </row>
-    <row r="348" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348" s="3"/>
       <c r="B348" s="4"/>
       <c r="C348" s="4"/>
       <c r="D348" s="4"/>
     </row>
-    <row r="349" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A349" s="3"/>
       <c r="B349" s="4"/>
       <c r="C349" s="4"/>
       <c r="D349" s="4"/>
     </row>
-    <row r="350" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350" s="3"/>
       <c r="B350" s="4"/>
       <c r="C350" s="4"/>
       <c r="D350" s="4"/>
     </row>
-    <row r="351" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A351" s="3"/>
       <c r="B351" s="4"/>
       <c r="C351" s="4"/>
       <c r="D351" s="4"/>
     </row>
-    <row r="352" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352" s="3"/>
       <c r="B352" s="4"/>
       <c r="C352" s="4"/>
       <c r="D352" s="4"/>
     </row>
-    <row r="353" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353" s="3"/>
       <c r="B353" s="4"/>
       <c r="C353" s="4"/>
       <c r="D353" s="4"/>
     </row>
-    <row r="354" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354" s="3"/>
       <c r="B354" s="4"/>
       <c r="C354" s="4"/>
       <c r="D354" s="4"/>
     </row>
-    <row r="355" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355" s="3"/>
       <c r="B355" s="4"/>
       <c r="C355" s="4"/>
       <c r="D355" s="4"/>
     </row>
-    <row r="356" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356" s="3"/>
       <c r="B356" s="4"/>
       <c r="C356" s="4"/>
       <c r="D356" s="4"/>
     </row>
-    <row r="357" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357" s="3"/>
       <c r="B357" s="4"/>
       <c r="C357" s="4"/>
       <c r="D357" s="4"/>
     </row>
-    <row r="358" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358" s="3"/>
       <c r="B358" s="4"/>
       <c r="C358" s="4"/>
       <c r="D358" s="4"/>
     </row>
-    <row r="359" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359" s="3"/>
       <c r="B359" s="4"/>
       <c r="C359" s="4"/>
       <c r="D359" s="4"/>
     </row>
-    <row r="360" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360" s="3"/>
       <c r="B360" s="4"/>
       <c r="C360" s="4"/>
       <c r="D360" s="4"/>
     </row>
-    <row r="361" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361" s="3"/>
       <c r="B361" s="4"/>
       <c r="C361" s="4"/>
       <c r="D361" s="4"/>
     </row>
-    <row r="362" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362" s="3"/>
       <c r="B362" s="4"/>
       <c r="C362" s="4"/>
       <c r="D362" s="4"/>
     </row>
-    <row r="363" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363" s="3"/>
       <c r="B363" s="4"/>
       <c r="C363" s="4"/>
       <c r="D363" s="4"/>
     </row>
-    <row r="364" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364" s="3"/>
       <c r="B364" s="4"/>
       <c r="C364" s="4"/>
       <c r="D364" s="4"/>
     </row>
-    <row r="365" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365" s="3"/>
       <c r="B365" s="4"/>
       <c r="C365" s="4"/>
       <c r="D365" s="4"/>
     </row>
-    <row r="366" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366" s="3"/>
       <c r="B366" s="4"/>
       <c r="C366" s="4"/>
       <c r="D366" s="4"/>
     </row>
-    <row r="367" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367" s="3"/>
       <c r="B367" s="4"/>
       <c r="C367" s="4"/>
       <c r="D367" s="4"/>
     </row>
-    <row r="368" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368" s="3"/>
       <c r="B368" s="4"/>
       <c r="C368" s="4"/>
       <c r="D368" s="4"/>
     </row>
-    <row r="369" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A369" s="3"/>
       <c r="B369" s="4"/>
       <c r="C369" s="4"/>
       <c r="D369" s="4"/>
     </row>
-    <row r="370" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A370" s="3"/>
       <c r="B370" s="4"/>
       <c r="C370" s="4"/>
       <c r="D370" s="4"/>
     </row>
-    <row r="371" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A371" s="3"/>
       <c r="B371" s="4"/>
       <c r="C371" s="4"/>
       <c r="D371" s="4"/>
     </row>
-    <row r="372" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A372" s="3"/>
       <c r="B372" s="4"/>
       <c r="C372" s="4"/>
       <c r="D372" s="4"/>
     </row>
-    <row r="373" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A373" s="3"/>
       <c r="B373" s="4"/>
       <c r="C373" s="4"/>
       <c r="D373" s="4"/>
     </row>
-    <row r="374" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A374" s="3"/>
       <c r="B374" s="4"/>
       <c r="C374" s="4"/>
       <c r="D374" s="4"/>
     </row>
-    <row r="375" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A375" s="3"/>
       <c r="B375" s="4"/>
       <c r="C375" s="4"/>
       <c r="D375" s="4"/>
     </row>
-    <row r="376" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A376" s="3"/>
       <c r="B376" s="4"/>
       <c r="C376" s="4"/>
       <c r="D376" s="4"/>
     </row>
-    <row r="377" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A377" s="3"/>
       <c r="B377" s="3"/>
       <c r="C377" s="4"/>
       <c r="D377" s="4"/>
     </row>
-    <row r="378" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A378" s="3"/>
       <c r="B378" s="3"/>
       <c r="C378" s="4"/>
       <c r="D378" s="4"/>
     </row>
-    <row r="379" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A379" s="3"/>
       <c r="B379" s="4"/>
       <c r="C379" s="4"/>
       <c r="D379" s="4"/>
     </row>
-    <row r="380" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A380" s="3"/>
       <c r="B380" s="4"/>
       <c r="C380" s="4"/>
       <c r="D380" s="4"/>
     </row>
-    <row r="381" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A381" s="3"/>
       <c r="B381" s="4"/>
       <c r="C381" s="4"/>
       <c r="D381" s="4"/>
     </row>
-    <row r="382" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A382" s="3"/>
       <c r="B382" s="4"/>
       <c r="C382" s="4"/>
       <c r="D382" s="4"/>
     </row>
-    <row r="383" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A383" s="3"/>
       <c r="B383" s="4"/>
       <c r="C383" s="4"/>
       <c r="D383" s="4"/>
     </row>
-    <row r="384" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A384" s="3"/>
       <c r="B384" s="4"/>
       <c r="C384" s="4"/>
       <c r="D384" s="4"/>
     </row>
-    <row r="385" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A385" s="3"/>
       <c r="B385" s="4"/>
       <c r="C385" s="4"/>
       <c r="D385" s="4"/>
     </row>
-    <row r="386" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386" s="3"/>
       <c r="B386" s="4"/>
       <c r="C386" s="4"/>
       <c r="D386" s="4"/>
     </row>
-    <row r="387" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A387" s="3"/>
       <c r="B387" s="4"/>
       <c r="C387" s="4"/>
       <c r="D387" s="4"/>
     </row>
-    <row r="388" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A388" s="3"/>
       <c r="B388" s="4"/>
       <c r="C388" s="4"/>
       <c r="D388" s="4"/>
     </row>
-    <row r="389" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A389" s="3"/>
       <c r="B389" s="4"/>
       <c r="C389" s="4"/>
       <c r="D389" s="4"/>
     </row>
-    <row r="390" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A390" s="3"/>
       <c r="B390" s="4"/>
       <c r="C390" s="4"/>
       <c r="D390" s="4"/>
     </row>
-    <row r="391" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A391" s="3"/>
       <c r="B391" s="4"/>
       <c r="C391" s="4"/>
       <c r="D391" s="4"/>
     </row>
-    <row r="392" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A392" s="3"/>
       <c r="B392" s="4"/>
       <c r="C392" s="4"/>
       <c r="D392" s="4"/>
     </row>
-    <row r="393" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A393" s="3"/>
       <c r="B393" s="4"/>
       <c r="C393" s="4"/>
       <c r="D393" s="4"/>
     </row>
-    <row r="394" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A394" s="3"/>
       <c r="B394" s="4"/>
       <c r="C394" s="4"/>
       <c r="D394" s="4"/>
     </row>
-    <row r="395" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A395" s="3"/>
       <c r="B395" s="4"/>
       <c r="C395" s="4"/>
       <c r="D395" s="4"/>
     </row>
-    <row r="396" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A396" s="3"/>
       <c r="B396" s="4"/>
       <c r="C396" s="4"/>
       <c r="D396" s="4"/>
     </row>
-    <row r="397" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A397" s="3"/>
       <c r="B397" s="4"/>
       <c r="C397" s="4"/>
       <c r="D397" s="4"/>
     </row>
-    <row r="398" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A398" s="3"/>
       <c r="B398" s="4"/>
       <c r="C398" s="4"/>
       <c r="D398" s="4"/>
     </row>
-    <row r="399" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A399" s="3"/>
       <c r="B399" s="4"/>
       <c r="C399" s="4"/>
       <c r="D399" s="4"/>
     </row>
-    <row r="400" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A400" s="3"/>
       <c r="B400" s="4"/>
       <c r="C400" s="4"/>
       <c r="D400" s="4"/>
     </row>
-    <row r="401" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A401" s="3"/>
       <c r="B401" s="4"/>
       <c r="C401" s="4"/>
       <c r="D401" s="4"/>
     </row>
-    <row r="402" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A402" s="3"/>
       <c r="B402" s="4"/>
       <c r="C402" s="4"/>
       <c r="D402" s="4"/>
     </row>
-    <row r="403" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A403" s="3"/>
       <c r="B403" s="4"/>
       <c r="C403" s="4"/>
       <c r="D403" s="4"/>
     </row>
-    <row r="404" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A404" s="3"/>
       <c r="B404" s="4"/>
       <c r="C404" s="4"/>
       <c r="D404" s="4"/>
     </row>
-    <row r="405" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A405" s="3"/>
       <c r="B405" s="4"/>
       <c r="C405" s="4"/>
       <c r="D405" s="4"/>
     </row>
-    <row r="406" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A406" s="3"/>
       <c r="B406" s="4"/>
       <c r="C406" s="4"/>
       <c r="D406" s="4"/>
     </row>
-    <row r="407" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A407" s="3"/>
       <c r="B407" s="4"/>
       <c r="C407" s="4"/>
       <c r="D407" s="4"/>
     </row>
-    <row r="408" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A408" s="3"/>
       <c r="B408" s="4"/>
       <c r="C408" s="4"/>
       <c r="D408" s="4"/>
     </row>
-    <row r="409" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A409" s="3"/>
       <c r="B409" s="4"/>
       <c r="C409" s="4"/>
       <c r="D409" s="4"/>
     </row>
-    <row r="410" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A410" s="3"/>
       <c r="B410" s="4"/>
       <c r="C410" s="4"/>
       <c r="D410" s="4"/>
     </row>
-    <row r="411" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A411" s="3"/>
       <c r="B411" s="4"/>
       <c r="C411" s="4"/>
       <c r="D411" s="4"/>
     </row>
-    <row r="412" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A412" s="3"/>
       <c r="B412" s="4"/>
       <c r="C412" s="4"/>
       <c r="D412" s="4"/>
     </row>
-    <row r="413" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A413" s="3"/>
       <c r="B413" s="4"/>
       <c r="C413" s="4"/>
       <c r="D413" s="4"/>
     </row>
-    <row r="414" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A414" s="3"/>
       <c r="B414" s="4"/>
       <c r="C414" s="4"/>
       <c r="D414" s="4"/>
     </row>
-    <row r="415" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A415" s="3"/>
       <c r="B415" s="4"/>
       <c r="C415" s="4"/>
       <c r="D415" s="4"/>
     </row>
-    <row r="416" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A416" s="3"/>
       <c r="B416" s="4"/>
       <c r="C416" s="4"/>
       <c r="D416" s="4"/>
     </row>
-    <row r="417" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A417" s="3"/>
       <c r="B417" s="4"/>
       <c r="C417" s="4"/>
       <c r="D417" s="4"/>
     </row>
-    <row r="418" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A418" s="3"/>
       <c r="B418" s="4"/>
       <c r="C418" s="4"/>
       <c r="D418" s="4"/>
     </row>
-    <row r="419" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A419" s="3"/>
       <c r="B419" s="4"/>
       <c r="C419" s="4"/>
       <c r="D419" s="4"/>
     </row>
-    <row r="420" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A420" s="3"/>
       <c r="B420" s="4"/>
       <c r="C420" s="4"/>
       <c r="D420" s="4"/>
     </row>
-    <row r="421" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A421" s="3"/>
       <c r="B421" s="4"/>
       <c r="C421" s="4"/>
       <c r="D421" s="4"/>
     </row>
-    <row r="422" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A422" s="3"/>
       <c r="B422" s="4"/>
       <c r="C422" s="4"/>
       <c r="D422" s="4"/>
     </row>
-    <row r="423" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A423" s="3"/>
       <c r="B423" s="4"/>
       <c r="C423" s="4"/>
       <c r="D423" s="4"/>
     </row>
-    <row r="424" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A424" s="3"/>
       <c r="B424" s="4"/>
       <c r="C424" s="4"/>
       <c r="D424" s="4"/>
     </row>
-    <row r="425" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A425" s="3"/>
       <c r="B425" s="4"/>
       <c r="C425" s="4"/>
       <c r="D425" s="4"/>
     </row>
-    <row r="426" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A426" s="3"/>
       <c r="B426" s="4"/>
       <c r="C426" s="4"/>
       <c r="D426" s="4"/>
     </row>
-    <row r="427" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A427" s="3"/>
       <c r="B427" s="4"/>
       <c r="C427" s="4"/>
       <c r="D427" s="4"/>
     </row>
-    <row r="428" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A428" s="3"/>
       <c r="B428" s="4"/>
       <c r="C428" s="4"/>
       <c r="D428" s="4"/>
     </row>
-    <row r="429" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A429" s="3"/>
       <c r="B429" s="4"/>
       <c r="C429" s="4"/>
       <c r="D429" s="4"/>
     </row>
-    <row r="430" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A430" s="3"/>
       <c r="B430" s="4"/>
       <c r="C430" s="4"/>
       <c r="D430" s="4"/>
     </row>
-    <row r="431" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A431" s="3"/>
       <c r="B431" s="4"/>
       <c r="C431" s="4"/>
       <c r="D431" s="4"/>
     </row>
-    <row r="432" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A432" s="3"/>
       <c r="B432" s="4"/>
       <c r="C432" s="4"/>
       <c r="D432" s="4"/>
     </row>
-    <row r="433" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A433" s="3"/>
       <c r="B433" s="4"/>
       <c r="C433" s="4"/>
       <c r="D433" s="4"/>
     </row>
-    <row r="434" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A434" s="3"/>
       <c r="B434" s="4"/>
       <c r="C434" s="4"/>
       <c r="D434" s="4"/>
     </row>
-    <row r="435" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A435" s="3"/>
       <c r="B435" s="4"/>
       <c r="C435" s="4"/>
       <c r="D435" s="4"/>
     </row>
-    <row r="436" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A436" s="3"/>
       <c r="B436" s="4"/>
       <c r="C436" s="4"/>
       <c r="D436" s="4"/>
     </row>
-    <row r="437" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A437" s="3"/>
       <c r="B437" s="4"/>
       <c r="C437" s="4"/>
       <c r="D437" s="4"/>
     </row>
-    <row r="438" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A438" s="3"/>
       <c r="B438" s="4"/>
       <c r="C438" s="4"/>
       <c r="D438" s="4"/>
     </row>
-    <row r="439" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A439" s="3"/>
       <c r="B439" s="4"/>
       <c r="C439" s="4"/>
       <c r="D439" s="4"/>
     </row>
-    <row r="440" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A440" s="3"/>
       <c r="B440" s="4"/>
       <c r="C440" s="4"/>
       <c r="D440" s="4"/>
     </row>
-    <row r="441" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A441" s="3"/>
       <c r="B441" s="4"/>
       <c r="C441" s="4"/>
       <c r="D441" s="4"/>
     </row>
-    <row r="442" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A442" s="3"/>
       <c r="B442" s="4"/>
       <c r="C442" s="4"/>
       <c r="D442" s="4"/>
     </row>
-    <row r="443" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A443" s="3"/>
       <c r="B443" s="4"/>
       <c r="C443" s="4"/>
       <c r="D443" s="4"/>
     </row>
-    <row r="444" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A444" s="3"/>
       <c r="B444" s="4"/>
       <c r="C444" s="4"/>
       <c r="D444" s="4"/>
     </row>
-    <row r="445" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A445" s="3"/>
       <c r="B445" s="4"/>
       <c r="C445" s="4"/>
       <c r="D445" s="4"/>
     </row>
-    <row r="446" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A446" s="3"/>
       <c r="B446" s="4"/>
       <c r="C446" s="4"/>
       <c r="D446" s="4"/>
     </row>
-    <row r="447" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A447" s="3"/>
       <c r="B447" s="4"/>
       <c r="C447" s="4"/>
       <c r="D447" s="4"/>
     </row>
-    <row r="448" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A448" s="3"/>
       <c r="B448" s="4"/>
       <c r="C448" s="4"/>
       <c r="D448" s="4"/>
     </row>
-    <row r="449" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A449" s="3"/>
       <c r="B449" s="4"/>
       <c r="C449" s="4"/>
       <c r="D449" s="4"/>
     </row>
-    <row r="450" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A450" s="3"/>
       <c r="B450" s="4"/>
       <c r="C450" s="4"/>
       <c r="D450" s="4"/>
     </row>
-    <row r="451" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A451" s="3"/>
       <c r="B451" s="4"/>
       <c r="C451" s="4"/>
       <c r="D451" s="4"/>
     </row>
-    <row r="452" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A452" s="3"/>
       <c r="B452" s="3"/>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
     </row>
-    <row r="453" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A453" s="3"/>
       <c r="B453" s="4"/>
       <c r="C453" s="4"/>
       <c r="D453" s="4"/>
     </row>
-    <row r="454" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A454" s="3"/>
       <c r="B454" s="4"/>
       <c r="C454" s="4"/>
       <c r="D454" s="4"/>
     </row>
-    <row r="455" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A455" s="3"/>
       <c r="B455" s="4"/>
       <c r="C455" s="4"/>
       <c r="D455" s="4"/>
     </row>
-    <row r="456" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A456" s="3"/>
       <c r="B456" s="4"/>
       <c r="C456" s="4"/>
       <c r="D456" s="4"/>
     </row>
-    <row r="457" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A457" s="3"/>
       <c r="B457" s="4"/>
       <c r="C457" s="4"/>
       <c r="D457" s="4"/>
     </row>
-    <row r="458" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A458" s="3"/>
       <c r="B458" s="4"/>
       <c r="C458" s="4"/>
       <c r="D458" s="4"/>
     </row>
-    <row r="459" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A459" s="3"/>
       <c r="B459" s="4"/>
       <c r="C459" s="4"/>
       <c r="D459" s="4"/>
     </row>
-    <row r="460" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A460" s="3"/>
       <c r="B460" s="4"/>
       <c r="C460" s="4"/>
       <c r="D460" s="4"/>
     </row>
-    <row r="461" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A461" s="3"/>
       <c r="B461" s="4"/>
       <c r="C461" s="4"/>
       <c r="D461" s="4"/>
     </row>
-    <row r="462" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A462" s="3"/>
       <c r="B462" s="4"/>
       <c r="C462" s="4"/>
       <c r="D462" s="4"/>
     </row>
-    <row r="463" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A463" s="3"/>
       <c r="B463" s="4"/>
       <c r="C463" s="4"/>
       <c r="D463" s="4"/>
     </row>
-    <row r="464" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A464" s="3"/>
       <c r="B464" s="4"/>
       <c r="C464" s="4"/>
       <c r="D464" s="4"/>
     </row>
-    <row r="465" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A465" s="3"/>
       <c r="B465" s="3"/>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
     </row>
-    <row r="466" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A466" s="3"/>
       <c r="B466" s="3"/>
       <c r="C466" s="3"/>
       <c r="D466" s="3"/>
     </row>
-    <row r="467" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A467" s="3"/>
       <c r="B467" s="3"/>
       <c r="C467" s="3"/>
       <c r="D467" s="3"/>
     </row>
-    <row r="468" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A468" s="3"/>
       <c r="B468" s="3"/>
       <c r="C468" s="3"/>
       <c r="D468" s="3"/>
     </row>
-    <row r="469" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A469" s="3"/>
       <c r="B469" s="3"/>
       <c r="C469" s="3"/>
       <c r="D469" s="3"/>
     </row>
-    <row r="470" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A470" s="3"/>
       <c r="B470" s="4"/>
       <c r="C470" s="4"/>
       <c r="D470" s="4"/>
     </row>
-    <row r="471" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A471" s="3"/>
       <c r="B471" s="4"/>
       <c r="C471" s="4"/>
       <c r="D471" s="4"/>
     </row>
-    <row r="472" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A472" s="3"/>
       <c r="B472" s="4"/>
       <c r="C472" s="4"/>
       <c r="D472" s="4"/>
     </row>
-    <row r="473" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A473" s="3"/>
       <c r="B473" s="4"/>
       <c r="C473" s="4"/>
       <c r="D473" s="4"/>
     </row>
-    <row r="474" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A474" s="3"/>
       <c r="B474" s="4"/>
       <c r="C474" s="4"/>
       <c r="D474" s="4"/>
     </row>
-    <row r="475" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A475" s="3"/>
       <c r="B475" s="4"/>
       <c r="C475" s="4"/>
       <c r="D475" s="4"/>
     </row>
-    <row r="476" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A476" s="3"/>
       <c r="B476" s="4"/>
       <c r="C476" s="4"/>
       <c r="D476" s="4"/>
     </row>
-    <row r="477" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A477" s="3"/>
       <c r="B477" s="4"/>
       <c r="C477" s="4"/>
       <c r="D477" s="4"/>
     </row>
-    <row r="478" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A478" s="3"/>
       <c r="B478" s="4"/>
       <c r="C478" s="4"/>
       <c r="D478" s="4"/>
     </row>
-    <row r="479" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A479" s="3"/>
       <c r="B479" s="4"/>
       <c r="C479" s="4"/>
       <c r="D479" s="4"/>
     </row>
-    <row r="480" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A480" s="3"/>
       <c r="B480" s="4"/>
       <c r="C480" s="4"/>
       <c r="D480" s="4"/>
     </row>
-    <row r="481" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A481" s="3"/>
       <c r="B481" s="4"/>
       <c r="C481" s="4"/>
       <c r="D481" s="4"/>
     </row>
-    <row r="482" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A482" s="3"/>
       <c r="B482" s="4"/>
       <c r="C482" s="4"/>
       <c r="D482" s="4"/>
     </row>
-    <row r="483" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A483" s="3"/>
       <c r="B483" s="4"/>
       <c r="C483" s="4"/>
       <c r="D483" s="4"/>
     </row>
-    <row r="484" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A484" s="3"/>
       <c r="B484" s="4"/>
       <c r="C484" s="4"/>
       <c r="D484" s="4"/>
     </row>
-    <row r="485" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A485" s="3"/>
       <c r="B485" s="3"/>
       <c r="C485" s="3"/>
       <c r="D485" s="3"/>
     </row>
-    <row r="486" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A486" s="3"/>
       <c r="B486" s="3"/>
       <c r="C486" s="3"/>

</xml_diff>

<commit_message>
- add chinese - update minimum insurance amount - update policy table of contents
</commit_message>
<xml_diff>
--- a/src/locales/languages.xlsx
+++ b/src/locales/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/projects/hieunm/tax-calculator/src/locales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EA5C79-E14B-0942-B775-3B3F965ABFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794FC8B0-31AE-DA4C-9552-2F6FB0F9010E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="27320" windowHeight="14240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="225">
   <si>
     <t>Key</t>
   </si>
@@ -586,13 +586,127 @@
   </si>
   <si>
     <t>급여 및 세금 세부 정보</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>必填</t>
+  </si>
+  <si>
+    <t>個人所得稅計算器</t>
+  </si>
+  <si>
+    <t>收入</t>
+  </si>
+  <si>
+    <t>輸入收入</t>
+  </si>
+  <si>
+    <t>受扶養人</t>
+  </si>
+  <si>
+    <t>輸入受扶養人</t>
+  </si>
+  <si>
+    <t>繳費等級</t>
+  </si>
+  <si>
+    <t>以正式工資計算</t>
+  </si>
+  <si>
+    <t>其他</t>
+  </si>
+  <si>
+    <t>繳費金額</t>
+  </si>
+  <si>
+    <t>至少 {0}₫</t>
+  </si>
+  <si>
+    <t>目標工資類型</t>
+  </si>
+  <si>
+    <t>淨收入</t>
+  </si>
+  <si>
+    <t>總收入</t>
+  </si>
+  <si>
+    <t>計算至 {0}</t>
+  </si>
+  <si>
+    <t>薪資和稅務詳情</t>
+  </si>
+  <si>
+    <t>總收入為 {0}₫</t>
+  </si>
+  <si>
+    <t>已繳保險費為 {0}₫</t>
+  </si>
+  <si>
+    <t>稅前收入為 {0}₫</t>
+  </si>
+  <si>
+    <t>應稅所得為 {0}₫</t>
+  </si>
+  <si>
+    <t>稅額為 {0}₫</t>
+  </si>
+  <si>
+    <t>淨收入為 {0}₫</t>
+  </si>
+  <si>
+    <t>語言</t>
+  </si>
+  <si>
+    <t>深色模式</t>
+  </si>
+  <si>
+    <t>關閉</t>
+  </si>
+  <si>
+    <t>個人扣除額</t>
+  </si>
+  <si>
+    <t>受扶養人扣除額</t>
+  </si>
+  <si>
+    <t>保險費率</t>
+  </si>
+  <si>
+    <t>最低保險基數</t>
+  </si>
+  <si>
+    <t>個人所得稅政策</t>
+  </si>
+  <si>
+    <t>04/2007/QH12 號 法律</t>
+  </si>
+  <si>
+    <t>第 954/2020/UBTVQH14 號決議</t>
+  </si>
+  <si>
+    <t>第 110/2025/UBTVQH15 號決議</t>
+  </si>
+  <si>
+    <t>稅收政策詳情</t>
+  </si>
+  <si>
+    <t>稅級</t>
+  </si>
+  <si>
+    <t>稅階</t>
+  </si>
+  <si>
+    <t>稅率</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -627,6 +741,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -648,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -668,6 +788,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,11 +982,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E486"/>
+  <dimension ref="A1:F486"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -875,9 +996,10 @@
     <col min="3" max="3" width="42.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="30" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -893,8 +1015,11 @@
       <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -910,8 +1035,11 @@
       <c r="E2" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F2" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -927,8 +1055,11 @@
       <c r="E3" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F3" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -944,8 +1075,11 @@
       <c r="E4" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F4" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -961,8 +1095,11 @@
       <c r="E5" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F5" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -978,8 +1115,11 @@
       <c r="E6" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F6" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -995,8 +1135,11 @@
       <c r="E7" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F7" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1012,8 +1155,11 @@
       <c r="E8" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F8" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1029,8 +1175,11 @@
       <c r="E9" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F9" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -1046,8 +1195,11 @@
       <c r="E10" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F10" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
@@ -1063,8 +1215,11 @@
       <c r="E11" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F11" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -1080,8 +1235,11 @@
       <c r="E12" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F12" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
@@ -1097,8 +1255,11 @@
       <c r="E13" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="F13" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -1114,8 +1275,11 @@
       <c r="E14" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="F14" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1131,8 +1295,11 @@
       <c r="E15" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F15" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
@@ -1148,8 +1315,11 @@
       <c r="E16" s="4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F16" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
@@ -1165,8 +1335,11 @@
       <c r="E17" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F17" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>110</v>
       </c>
@@ -1182,8 +1355,11 @@
       <c r="E18" s="4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F18" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>111</v>
       </c>
@@ -1199,8 +1375,11 @@
       <c r="E19" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F19" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>112</v>
       </c>
@@ -1216,8 +1395,11 @@
       <c r="E20" s="4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F20" s="7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>113</v>
       </c>
@@ -1233,8 +1415,11 @@
       <c r="E21" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F21" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>114</v>
       </c>
@@ -1250,8 +1435,11 @@
       <c r="E22" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F22" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>115</v>
       </c>
@@ -1267,8 +1455,11 @@
       <c r="E23" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F23" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>62</v>
       </c>
@@ -1284,8 +1475,11 @@
       <c r="E24" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F24" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>66</v>
       </c>
@@ -1301,8 +1495,11 @@
       <c r="E25" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F25" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>70</v>
       </c>
@@ -1318,8 +1515,11 @@
       <c r="E26" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F26" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>74</v>
       </c>
@@ -1335,8 +1535,11 @@
       <c r="E27" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F27" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>78</v>
       </c>
@@ -1352,8 +1555,11 @@
       <c r="E28" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F28" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>82</v>
       </c>
@@ -1369,8 +1575,11 @@
       <c r="E29" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F29" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>86</v>
       </c>
@@ -1386,8 +1595,11 @@
       <c r="E30" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F30" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>90</v>
       </c>
@@ -1403,8 +1615,11 @@
       <c r="E31" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F31" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>159</v>
       </c>
@@ -1420,8 +1635,11 @@
       <c r="E32" s="4" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F32" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>162</v>
       </c>
@@ -1437,8 +1655,11 @@
       <c r="E33" s="4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F33" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>163</v>
       </c>
@@ -1454,8 +1675,11 @@
       <c r="E34" s="4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F34" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>164</v>
       </c>
@@ -1471,8 +1695,11 @@
       <c r="E35" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F35" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>178</v>
       </c>
@@ -1488,8 +1715,11 @@
       <c r="E36" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F36" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>155</v>
       </c>
@@ -1505,8 +1735,11 @@
       <c r="E37" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F37" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>153</v>
       </c>
@@ -1522,8 +1755,11 @@
       <c r="E38" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F38" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>154</v>
       </c>
@@ -1539,8 +1775,11 @@
       <c r="E39" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F39" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>94</v>
       </c>
@@ -1556,50 +1795,53 @@
       <c r="E40" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>

</xml_diff>